<commit_message>
Ready for testing rcot problem.
</commit_message>
<xml_diff>
--- a/default/2_sut_multi_year_rcot/concept.xlsx
+++ b/default/2_sut_multi_year_rcot/concept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\2_sut_multi_year_rcot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9486115-17B7-4E18-AA24-8DED9769AD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F93505-D581-48E7-B11A-CE6EF4C6D497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{0A3BC822-FD99-4F89-AC4E-FBD077FFAF78}"/>
+    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{0A3BC822-FD99-4F89-AC4E-FBD077FFAF78}"/>
   </bookViews>
   <sheets>
     <sheet name="multi-year" sheetId="6" r:id="rId1"/>
@@ -174,9 +174,6 @@
     <t>X - d*Q' == 0</t>
   </si>
   <si>
-    <t>Q' - u*X - Y == 0</t>
-  </si>
-  <si>
     <t>i_t1</t>
   </si>
   <si>
@@ -198,13 +195,16 @@
     <t>electricity</t>
   </si>
   <si>
-    <t>Q_agg</t>
-  </si>
-  <si>
     <t>I_ff</t>
   </si>
   <si>
     <t>X &lt;= X_max</t>
+  </si>
+  <si>
+    <t>Q_agg - u*X - Y == 0</t>
+  </si>
+  <si>
+    <t>Q_agg == I_ff * Q'</t>
   </si>
 </sst>
 </file>
@@ -760,8 +760,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -852,7 +852,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -900,7 +900,7 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="G7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J7" t="s">
         <v>21</v>
@@ -912,18 +912,18 @@
         <v>1.2</v>
       </c>
       <c r="S7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Y7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
         <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
@@ -1003,10 +1003,10 @@
         <v>32</v>
       </c>
       <c r="AE9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AG9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.35">
@@ -1141,7 +1141,7 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1196,7 +1196,7 @@
         <v>11727.644400000001</v>
       </c>
       <c r="T17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
@@ -1242,7 +1242,7 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="M29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Issue on reindexing when generating cvxpy variables solved (see issue #23 on github)
</commit_message>
<xml_diff>
--- a/default/2_sut_multi_year_rcot/concept.xlsx
+++ b/default/2_sut_multi_year_rcot/concept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\2_sut_multi_year_rcot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F93505-D581-48E7-B11A-CE6EF4C6D497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1300F95A-F3B5-46BA-90A9-37F232F60E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{0A3BC822-FD99-4F89-AC4E-FBD077FFAF78}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{0A3BC822-FD99-4F89-AC4E-FBD077FFAF78}"/>
   </bookViews>
   <sheets>
     <sheet name="multi-year" sheetId="6" r:id="rId1"/>
@@ -758,10 +758,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B9C269-8EBE-47B7-80AA-01E8CD0CCD53}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AK30"/>
+  <dimension ref="A1:AK35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z23" sqref="Z23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,6 +776,7 @@
       <c r="A1" t="s">
         <v>13</v>
       </c>
+      <c r="L1" s="4"/>
       <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
@@ -899,17 +900,11 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="G7" t="s">
-        <v>40</v>
-      </c>
       <c r="J7" t="s">
         <v>21</v>
       </c>
       <c r="M7" t="s">
         <v>22</v>
-      </c>
-      <c r="N7" s="4">
-        <v>1.2</v>
       </c>
       <c r="S7" t="s">
         <v>43</v>
@@ -928,12 +923,6 @@
       <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="13">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13">
-        <v>1</v>
-      </c>
       <c r="J8" s="1">
         <v>0.1</v>
       </c>
@@ -944,23 +933,19 @@
         <v>100</v>
       </c>
       <c r="N8" s="5">
-        <f t="shared" ref="N8:Q8" si="0">M8*$N$7</f>
         <v>120</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="P8" s="5">
-        <f t="shared" si="0"/>
-        <v>172.79999999999998</v>
+        <v>173</v>
       </c>
       <c r="Q8" s="5">
-        <f t="shared" si="0"/>
-        <v>207.35999999999999</v>
+        <v>207</v>
       </c>
       <c r="S8" s="16">
-        <f t="array" ref="S8:W8">MMULT(G8:H8,TRANSPOSE(G16:H20))</f>
+        <f t="array" ref="S8:W8">MMULT(G35:H35,TRANSPOSE(G16:H20))</f>
         <v>111.11111</v>
       </c>
       <c r="T8" s="16">
@@ -970,10 +955,10 @@
         <v>154</v>
       </c>
       <c r="V8" s="16">
-        <v>177.8</v>
+        <v>178</v>
       </c>
       <c r="W8" s="16">
-        <v>207.36</v>
+        <v>207</v>
       </c>
       <c r="Y8" s="17">
         <f t="array" ref="Y8:AC8">S8:W8-MMULT(J8:K8,S10:W11)-M8:Q8</f>
@@ -1095,10 +1080,10 @@
         <v>54</v>
       </c>
       <c r="V11" s="20">
-        <v>127.8</v>
+        <v>128</v>
       </c>
       <c r="W11" s="20">
-        <v>207.36</v>
+        <v>207</v>
       </c>
       <c r="Y11" s="10">
         <v>0</v>
@@ -1193,7 +1178,7 @@
       </c>
       <c r="S17" s="6">
         <f t="array" ref="S17">MMULT(M30:Q30,MMULT(J23:K27,AE10:AE11))</f>
-        <v>11727.644400000001</v>
+        <v>11724.4444</v>
       </c>
       <c r="T17" t="s">
         <v>35</v>
@@ -1218,7 +1203,7 @@
         <v>50</v>
       </c>
       <c r="H19" s="20">
-        <v>127.8</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
@@ -1229,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="20">
-        <v>207.36</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
@@ -1285,7 +1270,7 @@
         <v>500</v>
       </c>
       <c r="K26" s="14">
-        <v>2556</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
@@ -1296,7 +1281,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="14">
-        <v>4147.2000000000007</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
@@ -1318,6 +1303,19 @@
         <v>1</v>
       </c>
       <c r="Q30" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G35" s="13">
+        <v>1</v>
+      </c>
+      <c r="H35" s="13">
         <v>1</v>
       </c>
     </row>

</xml_diff>